<commit_message>
Save QGIS 3.16 edits
</commit_message>
<xml_diff>
--- a/spreadsheetData/BuildingKey.xlsx
+++ b/spreadsheetData/BuildingKey.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAD\Documents\GIS-Data\MusserMaps\spreadsheetData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20D013C-E861-421C-87A9-52917E788F00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA8D8A2-A6AD-45C8-8D66-AB0D21832F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{4722393B-1945-4A20-9019-DC9F64DF1D3D}"/>
+    <workbookView xWindow="25080" yWindow="-495" windowWidth="29040" windowHeight="16440" xr2:uid="{4722393B-1945-4A20-9019-DC9F64DF1D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="198">
   <si>
     <t>D-2</t>
   </si>
@@ -141,15 +141,6 @@
     <t>Dan Beard Cabin</t>
   </si>
   <si>
-    <t>Tent site 1</t>
-  </si>
-  <si>
-    <t>Tent site 2</t>
-  </si>
-  <si>
-    <t>Tent site 3</t>
-  </si>
-  <si>
     <t>Knollbrook Lodge</t>
   </si>
   <si>
@@ -276,9 +267,6 @@
     <t>Long Lake Common Area</t>
   </si>
   <si>
-    <t>Lucius Maxwell Lodge</t>
-  </si>
-  <si>
     <t>D-A</t>
   </si>
   <si>
@@ -366,48 +354,6 @@
     <t>H-19</t>
   </si>
   <si>
-    <t>H-20</t>
-  </si>
-  <si>
-    <t>H-21</t>
-  </si>
-  <si>
-    <t>H-22</t>
-  </si>
-  <si>
-    <t>H-23</t>
-  </si>
-  <si>
-    <t>H-24</t>
-  </si>
-  <si>
-    <t>H-25</t>
-  </si>
-  <si>
-    <t>H-26</t>
-  </si>
-  <si>
-    <t>H-27</t>
-  </si>
-  <si>
-    <t>H-28</t>
-  </si>
-  <si>
-    <t>H-29</t>
-  </si>
-  <si>
-    <t>H-30</t>
-  </si>
-  <si>
-    <t>H-31</t>
-  </si>
-  <si>
-    <t>H-32</t>
-  </si>
-  <si>
-    <t>H-33</t>
-  </si>
-  <si>
     <t>H-34</t>
   </si>
   <si>
@@ -423,9 +369,6 @@
     <t>Perry Long Lodge</t>
   </si>
   <si>
-    <t>Teddy Lodge</t>
-  </si>
-  <si>
     <t>Park Lodge</t>
   </si>
   <si>
@@ -438,9 +381,6 @@
     <t>Korman Lodge</t>
   </si>
   <si>
-    <t>Falcon Campsite</t>
-  </si>
-  <si>
     <t>Gold Stag</t>
   </si>
   <si>
@@ -631,13 +571,61 @@
   </si>
   <si>
     <t>Delaware Tent site</t>
+  </si>
+  <si>
+    <t>Sleepy Hollow</t>
+  </si>
+  <si>
+    <t>Lucien Maxwell Lodge</t>
+  </si>
+  <si>
+    <t>Handicraft Pavilion</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Carlson Tent Site</t>
+  </si>
+  <si>
+    <t>Sutton Tent Site</t>
+  </si>
+  <si>
+    <t>Cozy Lodge</t>
+  </si>
+  <si>
+    <t>D-K</t>
+  </si>
+  <si>
+    <t>Thunderbird Rock</t>
+  </si>
+  <si>
+    <t>D-50</t>
+  </si>
+  <si>
+    <t>D-51</t>
+  </si>
+  <si>
+    <t>D-52</t>
+  </si>
+  <si>
+    <t>Patrol 8</t>
+  </si>
+  <si>
+    <t>Patrol 9</t>
+  </si>
+  <si>
+    <t>Patrol 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,6 +639,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -660,9 +655,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -672,8 +676,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,445 +996,564 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1BC538-7651-4FD0-ABC3-A9FDD64E892C}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:H19"/>
+      <selection activeCell="N1" sqref="N1:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="14" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" t="s">
-        <v>94</v>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J1" t="s">
-        <v>141</v>
+        <v>112</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="K1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N1" t="s">
-        <v>181</v>
+        <v>123</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="O1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>95</v>
+      <c r="C2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" t="s">
-        <v>142</v>
+        <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" t="s">
-        <v>183</v>
+        <v>124</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="O2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="P2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" t="s">
-        <v>96</v>
+      <c r="C3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="H3" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" t="s">
-        <v>149</v>
+        <v>189</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="K3" t="s">
-        <v>145</v>
-      </c>
-      <c r="N3" t="s">
-        <v>185</v>
+        <v>125</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="O3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="P3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>87</v>
+        <v>187</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" t="s">
-        <v>97</v>
+        <v>81</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="H4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J4" t="s">
-        <v>150</v>
+        <v>114</v>
+      </c>
+      <c r="I4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="K4" t="s">
-        <v>146</v>
-      </c>
-      <c r="N4" t="s">
-        <v>187</v>
+        <v>126</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="O4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="P4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
+        <v>188</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G5" t="s">
-        <v>98</v>
+        <v>64</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" t="s">
-        <v>151</v>
+        <v>115</v>
+      </c>
+      <c r="I5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="K5" t="s">
-        <v>147</v>
-      </c>
-      <c r="N5" t="s">
-        <v>189</v>
+        <v>127</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="O5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="P5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>80</v>
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" t="s">
-        <v>99</v>
+        <v>78</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" t="s">
-        <v>152</v>
+        <v>116</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="K6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" t="s">
-        <v>100</v>
+        <v>61</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
-      </c>
-      <c r="J7" t="s">
-        <v>153</v>
+        <v>117</v>
+      </c>
+      <c r="I7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="K7" t="s">
-        <v>140</v>
-      </c>
-      <c r="N7" t="s">
-        <v>191</v>
+        <v>120</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="O7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G8" t="s">
-        <v>101</v>
+        <v>85</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H8" t="s">
-        <v>137</v>
-      </c>
-      <c r="J8" t="s">
-        <v>154</v>
+        <v>120</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="K8" t="s">
-        <v>166</v>
-      </c>
-      <c r="N8" t="s">
-        <v>193</v>
+        <v>146</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="O8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" t="s">
-        <v>102</v>
+        <v>79</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="H9" t="s">
-        <v>138</v>
-      </c>
-      <c r="J9" t="s">
-        <v>155</v>
+        <v>118</v>
+      </c>
+      <c r="I9" t="s">
+        <v>185</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="K9" t="s">
-        <v>167</v>
-      </c>
-      <c r="N9" t="s">
-        <v>195</v>
+        <v>147</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="O9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" t="s">
-        <v>103</v>
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="H10" t="s">
-        <v>139</v>
-      </c>
-      <c r="J10" t="s">
-        <v>156</v>
+        <v>119</v>
+      </c>
+      <c r="I10" t="s">
+        <v>185</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="K10" t="s">
-        <v>168</v>
-      </c>
-      <c r="N10" t="s">
-        <v>196</v>
+        <v>148</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="O10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G11" t="s">
-        <v>104</v>
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="H11" t="s">
-        <v>173</v>
-      </c>
-      <c r="J11" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="I11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="K11" t="s">
-        <v>169</v>
-      </c>
-      <c r="N11" t="s">
-        <v>198</v>
+        <v>149</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="O11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" t="s">
-        <v>105</v>
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="H12" t="s">
-        <v>174</v>
-      </c>
-      <c r="J12" t="s">
-        <v>158</v>
+        <v>154</v>
+      </c>
+      <c r="I12" t="s">
+        <v>185</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="K12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>200</v>
-      </c>
-      <c r="G13" t="s">
-        <v>106</v>
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="H13" t="s">
-        <v>175</v>
-      </c>
-      <c r="J13" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="I13" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="K13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" t="s">
-        <v>107</v>
+        <v>182</v>
+      </c>
+      <c r="C14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="H14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J14" t="s">
-        <v>160</v>
+        <v>156</v>
+      </c>
+      <c r="I14" t="s">
+        <v>185</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="K14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" t="s">
-        <v>108</v>
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>185</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H15" t="s">
-        <v>177</v>
-      </c>
-      <c r="J15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="I15" t="s">
+        <v>185</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" t="s">
-        <v>109</v>
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="H16" t="s">
-        <v>178</v>
-      </c>
-      <c r="J16" t="s">
-        <v>162</v>
+        <v>158</v>
+      </c>
+      <c r="I16" t="s">
+        <v>185</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1434,16 +1561,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" t="s">
-        <v>110</v>
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>185</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="H17" t="s">
-        <v>179</v>
-      </c>
-      <c r="J17" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+      <c r="I17" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1451,16 +1584,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" t="s">
-        <v>111</v>
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>185</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="H18" t="s">
-        <v>180</v>
-      </c>
-      <c r="J18" t="s">
-        <v>164</v>
+        <v>160</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1468,13 +1604,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" t="s">
-        <v>112</v>
-      </c>
-      <c r="J19" t="s">
-        <v>165</v>
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1482,10 +1624,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" t="s">
-        <v>113</v>
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1493,10 +1641,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" t="s">
-        <v>114</v>
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>185</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H21" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1504,10 +1658,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" t="s">
-        <v>115</v>
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1515,10 +1675,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" t="s">
-        <v>116</v>
+        <v>51</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1526,10 +1689,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" t="s">
-        <v>117</v>
+        <v>184</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1537,10 +1703,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" t="s">
-        <v>118</v>
+        <v>52</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1548,10 +1717,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" t="s">
-        <v>119</v>
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>185</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1559,10 +1734,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" t="s">
-        <v>120</v>
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>185</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1570,10 +1751,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28" t="s">
-        <v>121</v>
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>185</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1581,10 +1768,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" t="s">
-        <v>122</v>
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>186</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1592,10 +1785,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" t="s">
-        <v>123</v>
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1603,10 +1802,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" t="s">
-        <v>124</v>
+        <v>58</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H31" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1614,91 +1816,122 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C32" t="s">
+        <v>185</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>185</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>185</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>185</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>183</v>
+      </c>
+      <c r="C37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="G35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>73</v>
       </c>
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>79</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:E7">
-    <sortCondition ref="D1:D7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:E10">
+    <sortCondition ref="D4:D10"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>